<commit_message>
fixed the UI and lines are now straight plus background image and stats func
</commit_message>
<xml_diff>
--- a/Random Walk Project.xlsx
+++ b/Random Walk Project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Josh\IntroToCS\Exercises\final_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D5784C-D09C-4E25-BF84-FE33E1796009}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2611C228-2182-42F3-89B6-556B2FAA2EC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{6628930F-D501-43E5-9EE2-90DEB523C066}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="33">
   <si>
     <t>Walker Class</t>
   </si>
@@ -50,9 +51,6 @@
     <t>Attributes</t>
   </si>
   <si>
-    <t>direction</t>
-  </si>
-  <si>
     <t>float</t>
   </si>
   <si>
@@ -86,9 +84,6 @@
     <t>Obstacles</t>
   </si>
   <si>
-    <t>size</t>
-  </si>
-  <si>
     <t>Simulation Class</t>
   </si>
   <si>
@@ -98,7 +93,49 @@
     <t>Statistics Class Methods</t>
   </si>
   <si>
-    <t>step_size</t>
+    <t>location</t>
+  </si>
+  <si>
+    <t>(int,int)</t>
+  </si>
+  <si>
+    <t>one_step_random_direction_Walker</t>
+  </si>
+  <si>
+    <t>Magic_Gate Class</t>
+  </si>
+  <si>
+    <t>random_step_random_direction</t>
+  </si>
+  <si>
+    <t>one_step_discrete_direction</t>
+  </si>
+  <si>
+    <t>destination</t>
+  </si>
+  <si>
+    <t>properties</t>
+  </si>
+  <si>
+    <t>direction- one of 8 directions</t>
+  </si>
+  <si>
+    <t>length</t>
+  </si>
+  <si>
+    <t>check intersections</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>defaults to 0</t>
   </si>
 </sst>
 </file>
@@ -471,16 +508,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{594F4202-A0FD-4075-AD0D-3EB1328AC1D7}">
   <dimension ref="B5:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="19.19921875" customWidth="1"/>
+    <col min="2" max="2" width="32.19921875" customWidth="1"/>
     <col min="3" max="3" width="23.86328125" customWidth="1"/>
     <col min="4" max="4" width="13.59765625" customWidth="1"/>
-    <col min="8" max="8" width="15.46484375" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" customWidth="1"/>
     <col min="10" max="11" width="12.6640625" customWidth="1"/>
     <col min="12" max="12" width="23.796875" customWidth="1"/>
     <col min="13" max="13" width="15.46484375" customWidth="1"/>
@@ -492,10 +529,10 @@
         <v>0</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.45">
@@ -518,57 +555,73 @@
         <v>2</v>
       </c>
       <c r="L7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="N7" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
         <v>4</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>5</v>
       </c>
-      <c r="D8" t="s">
-        <v>6</v>
-      </c>
       <c r="L8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
         <v>5</v>
       </c>
-      <c r="D9" t="s">
-        <v>6</v>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="B11" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B13" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>3</v>
@@ -579,33 +632,83 @@
       <c r="J15" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="L15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" t="s">
         <v>12</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>13</v>
       </c>
-      <c r="D16" t="s">
-        <v>14</v>
-      </c>
       <c r="H16" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="I16" t="s">
+        <v>19</v>
+      </c>
+      <c r="J16" t="s">
         <v>5</v>
       </c>
-      <c r="J16" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="8:10" x14ac:dyDescent="0.45">
+      <c r="L16" t="s">
+        <v>18</v>
+      </c>
+      <c r="M16" t="s">
+        <v>19</v>
+      </c>
+      <c r="N16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="H17" t="s">
+        <v>27</v>
+      </c>
+      <c r="L17" t="s">
+        <v>24</v>
+      </c>
+      <c r="M17" t="s">
+        <v>19</v>
+      </c>
+      <c r="N17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="H18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="B20" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="B21" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.45">
+      <c r="B22" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="H22" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="8:10" x14ac:dyDescent="0.45">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.45">
       <c r="H24" s="1" t="s">
         <v>3</v>
       </c>

</xml_diff>